<commit_message>
added images to reels
</commit_message>
<xml_diff>
--- a/Assignment2_SlotMachine/Assignment2_SlotMachine/buttons.xlsx
+++ b/Assignment2_SlotMachine/Assignment2_SlotMachine/buttons.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\centennialcollege\semester6\Web Game\COMP397-WebGameProgramming\Assignment2_SlotMachine\Assignment2_SlotMachine\assets\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\centennialcollege\semester6\Web Game\COMP397-WebGameProgramming\Assignment2_SlotMachine\Assignment2_SlotMachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Button</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>POWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reel0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reel1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reel2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -124,11 +136,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,10 +426,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -524,6 +540,57 @@
         <v>345</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2">
+        <v>71</v>
+      </c>
+      <c r="E7" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2">
+        <v>112</v>
+      </c>
+      <c r="D8" s="2">
+        <v>171</v>
+      </c>
+      <c r="E8" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>82</v>
+      </c>
+      <c r="C9" s="2">
+        <v>112</v>
+      </c>
+      <c r="D9" s="2">
+        <v>271</v>
+      </c>
+      <c r="E9" s="2">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>